<commit_message>
Task ID#: ITSN032 - Upload Bulik User - Excel & CSV
</commit_message>
<xml_diff>
--- a/JG_Prospect-New/JG_Prospect.web/UserFile/SalesSample.xlsx
+++ b/JG_Prospect-New/JG_Prospect.web/UserFile/SalesSample.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Designition">Sheet2!$B$3:$B$9</definedName>
+    <definedName name="Designitions">Sheet2!$B$3:$B$9</definedName>
+    <definedName name="Status">Sheet2!$D$3:$D$9</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Mc.Callum</t>
   </si>
@@ -67,21 +73,9 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Forman</t>
-  </si>
-  <si>
     <t>Applicant</t>
   </si>
   <si>
-    <t>Refer below details for creating excel document</t>
-  </si>
-  <si>
-    <t>Designitions:</t>
-  </si>
-  <si>
-    <t>Status:</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -119,13 +113,31 @@
   </si>
   <si>
     <t>Sr. Sales</t>
+  </si>
+  <si>
+    <t>Fnam</t>
+  </si>
+  <si>
+    <t>Lasntnam</t>
+  </si>
+  <si>
+    <t>The Comp</t>
+  </si>
+  <si>
+    <t>email@ee.com</t>
+  </si>
+  <si>
+    <t>emsiel@sadfl.com</t>
+  </si>
+  <si>
+    <t>The naot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,7 +185,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -185,6 +197,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -192,6 +206,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -238,7 +260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,9 +292,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,6 +327,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,14 +503,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
@@ -500,7 +524,7 @@
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -535,7 +559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" customHeight="1">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -564,103 +588,142 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <v>9848847624</v>
+      </c>
+      <c r="E3">
+        <v>545</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="6">
+        <v>42405</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="B5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J200">
+      <formula1>Designitions</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K199">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>